<commit_message>
correção do cronograma dia da reuniao ricardo ... colocando dentro da data que aconteceu realmente a apresentaçao
</commit_message>
<xml_diff>
--- a/CronogramaFinal.xlsx
+++ b/CronogramaFinal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afonso\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufprbr0-my.sharepoint.com/personal/afonso_campos_ufpr_br/Documents/Rprojetos/ApresentacaoPosdoc/finalposdoc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94125865-5334-477D-807A-9C42007A1946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{5B4F8F50-24CD-4CB5-A7E5-F14408EEFF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7495DE7D-EA90-4932-8C97-3BE0C249C5BF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>Resultados</t>
   </si>
   <si>
-    <t xml:space="preserve">Sessão Publica </t>
-  </si>
-  <si>
     <t>Revisão</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sessão Pública </t>
   </si>
 </sst>
 </file>
@@ -400,29 +400,30 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -439,10 +440,10 @@
         <v>43069</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -459,10 +460,10 @@
         <v>43434</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -479,10 +480,10 @@
         <v>43799</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -499,10 +500,10 @@
         <v>44165</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -519,10 +520,10 @@
         <v>44499</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -539,10 +540,10 @@
         <v>44681</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -559,10 +560,10 @@
         <v>43040</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -579,10 +580,10 @@
         <v>43160</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -599,10 +600,10 @@
         <v>43069</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -619,10 +620,10 @@
         <v>43434</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -639,10 +640,10 @@
         <v>43799</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -659,10 +660,10 @@
         <v>44165</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -679,10 +680,10 @@
         <v>44499</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -699,10 +700,10 @@
         <v>44681</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -719,10 +720,10 @@
         <v>43069</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -739,10 +740,10 @@
         <v>43281</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -759,10 +760,10 @@
         <v>43434</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -779,10 +780,10 @@
         <v>43646</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -799,10 +800,10 @@
         <v>43799</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -819,10 +820,10 @@
         <v>44165</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -839,18 +840,18 @@
         <v>44012</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="1">
         <v>42856</v>
@@ -859,18 +860,18 @@
         <v>43069</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1">
         <v>43101</v>
@@ -879,18 +880,18 @@
         <v>43434</v>
       </c>
       <c r="E24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" s="1">
         <v>43466</v>
@@ -899,18 +900,18 @@
         <v>43799</v>
       </c>
       <c r="E25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="1">
         <v>43831</v>
@@ -919,18 +920,18 @@
         <v>44165</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="1">
         <v>44197</v>
@@ -939,18 +940,18 @@
         <v>44499</v>
       </c>
       <c r="E27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="1">
         <v>44562</v>
@@ -959,30 +960,30 @@
         <v>44681</v>
       </c>
       <c r="E28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1">
-        <v>44682</v>
+        <v>44743</v>
       </c>
       <c r="D29" s="1">
-        <v>44711</v>
+        <v>44772</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste de layout apos a reuniao com o ricardo. falta apenas colocar mais algumas anotações.
</commit_message>
<xml_diff>
--- a/CronogramaFinal.xlsx
+++ b/CronogramaFinal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufprbr0-my.sharepoint.com/personal/afonso_campos_ufpr_br/Documents/Rprojetos/ApresentacaoPosdoc/finalposdoc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{5B4F8F50-24CD-4CB5-A7E5-F14408EEFF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7495DE7D-EA90-4932-8C97-3BE0C249C5BF}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{5B4F8F50-24CD-4CB5-A7E5-F14408EEFF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D04BF38E-AE0B-454B-B2B0-CE4042163D83}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="18">
   <si>
     <t xml:space="preserve">Análise </t>
   </si>
@@ -54,24 +54,6 @@
     <t>color</t>
   </si>
   <si>
-    <t>#F28E2B</t>
-  </si>
-  <si>
-    <t>#76B7B2</t>
-  </si>
-  <si>
-    <t>#59A14F</t>
-  </si>
-  <si>
-    <t>#EDC948</t>
-  </si>
-  <si>
-    <t>#B07AA1</t>
-  </si>
-  <si>
-    <t>#9C755F</t>
-  </si>
-  <si>
     <t>white</t>
   </si>
   <si>
@@ -79,16 +61,40 @@
   </si>
   <si>
     <t xml:space="preserve">Sessão Pública </t>
+  </si>
+  <si>
+    <t>#4B6043</t>
+  </si>
+  <si>
+    <t>#DDEAD1</t>
+  </si>
+  <si>
+    <t>#658354</t>
+  </si>
+  <si>
+    <t>#C7DDB5</t>
+  </si>
+  <si>
+    <t>#95BB72</t>
+  </si>
+  <si>
+    <t>#B3CF99</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -397,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52AB15C-D07F-4E18-AE45-9F3D52CED5F4}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,10 +446,10 @@
         <v>43069</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -460,10 +466,10 @@
         <v>43434</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -480,10 +486,10 @@
         <v>43799</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -500,10 +506,10 @@
         <v>44165</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -520,10 +526,10 @@
         <v>44499</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -540,10 +546,10 @@
         <v>44681</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -560,10 +566,10 @@
         <v>43040</v>
       </c>
       <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
         <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -580,10 +586,10 @@
         <v>43160</v>
       </c>
       <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
         <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -600,10 +606,10 @@
         <v>43069</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -620,10 +626,10 @@
         <v>43434</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -640,10 +646,10 @@
         <v>43799</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -660,10 +666,10 @@
         <v>44165</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -680,10 +686,10 @@
         <v>44499</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -700,10 +706,10 @@
         <v>44681</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -720,10 +726,10 @@
         <v>43069</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -740,10 +746,10 @@
         <v>43281</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -760,10 +766,10 @@
         <v>43434</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -780,10 +786,10 @@
         <v>43646</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -800,10 +806,10 @@
         <v>43799</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -820,10 +826,10 @@
         <v>44165</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -840,30 +846,30 @@
         <v>44012</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23" s="1">
-        <v>42856</v>
+        <v>44501</v>
       </c>
       <c r="D23" s="1">
-        <v>43069</v>
+        <v>44530</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -874,16 +880,16 @@
         <v>4</v>
       </c>
       <c r="C24" s="1">
-        <v>43101</v>
+        <v>42856</v>
       </c>
       <c r="D24" s="1">
-        <v>43434</v>
+        <v>43069</v>
       </c>
       <c r="E24" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -894,16 +900,16 @@
         <v>4</v>
       </c>
       <c r="C25" s="1">
-        <v>43466</v>
+        <v>43101</v>
       </c>
       <c r="D25" s="1">
-        <v>43799</v>
+        <v>43434</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -914,16 +920,16 @@
         <v>4</v>
       </c>
       <c r="C26" s="1">
-        <v>43831</v>
+        <v>43466</v>
       </c>
       <c r="D26" s="1">
-        <v>44165</v>
+        <v>43799</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -934,16 +940,16 @@
         <v>4</v>
       </c>
       <c r="C27" s="1">
-        <v>44197</v>
+        <v>43831</v>
       </c>
       <c r="D27" s="1">
-        <v>44499</v>
+        <v>44165</v>
       </c>
       <c r="E27" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -954,39 +960,60 @@
         <v>4</v>
       </c>
       <c r="C28" s="1">
-        <v>44562</v>
+        <v>44197</v>
       </c>
       <c r="D28" s="1">
-        <v>44681</v>
+        <v>44499</v>
       </c>
       <c r="E28" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1">
+        <v>44562</v>
+      </c>
+      <c r="D29" s="1">
+        <v>44681</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1">
+        <v>44743</v>
+      </c>
+      <c r="D30" s="1">
+        <v>44772</v>
+      </c>
+      <c r="E30" t="s">
         <v>17</v>
       </c>
-      <c r="B29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="1">
-        <v>44743</v>
-      </c>
-      <c r="D29" s="1">
-        <v>44772</v>
-      </c>
-      <c r="E29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" t="s">
-        <v>15</v>
+      <c r="F30" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adicionando as ultimas anotações antes da apresentação. grafico de cronograma tb foi ajustada.
</commit_message>
<xml_diff>
--- a/CronogramaFinal.xlsx
+++ b/CronogramaFinal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufprbr0-my.sharepoint.com/personal/afonso_campos_ufpr_br/Documents/Rprojetos/ApresentacaoPosdoc/finalposdoc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{5B4F8F50-24CD-4CB5-A7E5-F14408EEFF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D04BF38E-AE0B-454B-B2B0-CE4042163D83}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{5B4F8F50-24CD-4CB5-A7E5-F14408EEFF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88C8B3DD-D241-4E9D-BDAA-A93129F2C6C2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="1440" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="24">
   <si>
     <t xml:space="preserve">Análise </t>
   </si>
@@ -79,6 +79,24 @@
   </si>
   <si>
     <t>#B3CF99</t>
+  </si>
+  <si>
+    <t>Apresentação dos resultados obtidos sessão pública.</t>
+  </si>
+  <si>
+    <t>Revisão de literatura, estudo, desenvolvimento de protocolos de análise</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Análise de dados</t>
+  </si>
+  <si>
+    <t>Coleta  de dados dos ensaios</t>
+  </si>
+  <si>
+    <t>Interpretação dos resultados, escrita e submissão artigos</t>
+  </si>
+  <si>
+    <t>Apresentação dos resultados parciais obtidos em seminários e relatórios (anuais e final)</t>
   </si>
 </sst>
 </file>
@@ -405,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52AB15C-D07F-4E18-AE45-9F3D52CED5F4}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,19 +452,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1">
-        <v>43009</v>
+        <v>42856</v>
       </c>
       <c r="D2" s="1">
         <v>43069</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -454,10 +472,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1">
         <v>43101</v>
@@ -466,7 +484,7 @@
         <v>43434</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -474,10 +492,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1">
         <v>43466</v>
@@ -486,7 +504,7 @@
         <v>43799</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -494,10 +512,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1">
         <v>43831</v>
@@ -506,7 +524,7 @@
         <v>44165</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -514,10 +532,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1">
         <v>44197</v>
@@ -526,7 +544,7 @@
         <v>44499</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -534,10 +552,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1">
         <v>44562</v>
@@ -546,7 +564,7 @@
         <v>44681</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -554,59 +572,59 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1">
-        <v>42856</v>
+        <v>43009</v>
       </c>
       <c r="D8" s="1">
-        <v>43040</v>
+        <v>43069</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1">
         <v>43101</v>
       </c>
       <c r="D9" s="1">
-        <v>43160</v>
+        <v>43434</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1">
-        <v>43009</v>
+        <v>43466</v>
       </c>
       <c r="D10" s="1">
-        <v>43069</v>
+        <v>43799</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
@@ -614,19 +632,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1">
-        <v>43101</v>
+        <v>43831</v>
       </c>
       <c r="D11" s="1">
-        <v>43434</v>
+        <v>44165</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -634,19 +652,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1">
-        <v>43466</v>
+        <v>44197</v>
       </c>
       <c r="D12" s="1">
-        <v>43799</v>
+        <v>44499</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
         <v>9</v>
@@ -654,19 +672,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1">
-        <v>43831</v>
+        <v>44562</v>
       </c>
       <c r="D13" s="1">
-        <v>44165</v>
+        <v>44681</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
@@ -674,162 +692,162 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1">
-        <v>44197</v>
+        <v>42856</v>
       </c>
       <c r="D14" s="1">
-        <v>44499</v>
+        <v>43040</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1">
-        <v>44562</v>
+        <v>43101</v>
       </c>
       <c r="D15" s="1">
-        <v>44681</v>
+        <v>43160</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1">
-        <v>43040</v>
+        <v>43009</v>
       </c>
       <c r="D16" s="1">
         <v>43069</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1">
-        <v>43252</v>
+        <v>43101</v>
       </c>
       <c r="D17" s="1">
-        <v>43281</v>
+        <v>43434</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1">
-        <v>43405</v>
+        <v>43466</v>
       </c>
       <c r="D18" s="1">
-        <v>43434</v>
+        <v>43799</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1">
-        <v>43617</v>
+        <v>43831</v>
       </c>
       <c r="D19" s="1">
-        <v>43646</v>
+        <v>44165</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C20" s="1">
-        <v>43770</v>
+        <v>44197</v>
       </c>
       <c r="D20" s="1">
-        <v>43799</v>
+        <v>44499</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C21" s="1">
-        <v>44136</v>
+        <v>44562</v>
       </c>
       <c r="D21" s="1">
-        <v>44165</v>
+        <v>44681</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -837,13 +855,13 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1">
-        <v>43983</v>
+        <v>43040</v>
       </c>
       <c r="D22" s="1">
-        <v>44012</v>
+        <v>43069</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
@@ -857,13 +875,13 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1">
-        <v>44501</v>
+        <v>43252</v>
       </c>
       <c r="D23" s="1">
-        <v>44530</v>
+        <v>43281</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
@@ -874,122 +892,122 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C24" s="1">
-        <v>42856</v>
+        <v>43405</v>
       </c>
       <c r="D24" s="1">
-        <v>43069</v>
+        <v>43434</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C25" s="1">
-        <v>43101</v>
+        <v>43617</v>
       </c>
       <c r="D25" s="1">
-        <v>43434</v>
+        <v>43646</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1">
-        <v>43466</v>
+        <v>43770</v>
       </c>
       <c r="D26" s="1">
         <v>43799</v>
       </c>
       <c r="E26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C27" s="1">
-        <v>43831</v>
+        <v>44136</v>
       </c>
       <c r="D27" s="1">
         <v>44165</v>
       </c>
       <c r="E27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C28" s="1">
-        <v>44197</v>
+        <v>43983</v>
       </c>
       <c r="D28" s="1">
-        <v>44499</v>
+        <v>44012</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C29" s="1">
-        <v>44562</v>
+        <v>44501</v>
       </c>
       <c r="D29" s="1">
-        <v>44681</v>
+        <v>44530</v>
       </c>
       <c r="E29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -997,7 +1015,7 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C30" s="1">
         <v>44743</v>

</xml_diff>

<commit_message>
Acredito que seja a versao definitiva ... aponas alguns comentarios adicionados.
</commit_message>
<xml_diff>
--- a/CronogramaFinal.xlsx
+++ b/CronogramaFinal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufprbr0-my.sharepoint.com/personal/afonso_campos_ufpr_br/Documents/Rprojetos/ApresentacaoPosdoc/finalposdoc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{5B4F8F50-24CD-4CB5-A7E5-F14408EEFF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88C8B3DD-D241-4E9D-BDAA-A93129F2C6C2}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{5B4F8F50-24CD-4CB5-A7E5-F14408EEFF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0F52C07-1DE7-4477-9AAD-924ECF50EAD4}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="1440" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,8 +423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52AB15C-D07F-4E18-AE45-9F3D52CED5F4}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,42 +572,42 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1">
-        <v>43009</v>
+        <v>42856</v>
       </c>
       <c r="D8" s="1">
-        <v>43069</v>
+        <v>43040</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1">
         <v>43101</v>
       </c>
       <c r="D9" s="1">
-        <v>43434</v>
+        <v>43160</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -618,10 +618,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="1">
-        <v>43466</v>
+        <v>43009</v>
       </c>
       <c r="D10" s="1">
-        <v>43799</v>
+        <v>43069</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -638,10 +638,10 @@
         <v>20</v>
       </c>
       <c r="C11" s="1">
-        <v>43831</v>
+        <v>43101</v>
       </c>
       <c r="D11" s="1">
-        <v>44165</v>
+        <v>43434</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -658,10 +658,10 @@
         <v>20</v>
       </c>
       <c r="C12" s="1">
-        <v>44197</v>
+        <v>43466</v>
       </c>
       <c r="D12" s="1">
-        <v>44499</v>
+        <v>43799</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -678,10 +678,10 @@
         <v>20</v>
       </c>
       <c r="C13" s="1">
-        <v>44562</v>
+        <v>43831</v>
       </c>
       <c r="D13" s="1">
-        <v>44681</v>
+        <v>44165</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -692,42 +692,42 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="1">
-        <v>42856</v>
+        <v>44197</v>
       </c>
       <c r="D14" s="1">
-        <v>43040</v>
+        <v>44499</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1">
-        <v>43101</v>
+        <v>44562</v>
       </c>
       <c r="D15" s="1">
-        <v>43160</v>
+        <v>44681</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>